<commit_message>
Parts finder app initialized, parent layout created.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/RFID_file.xlsx
+++ b/app/src/main/assets/RFID_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kyotogakuen1.sharepoint.com/sites/24C11RFID/Shared Documents/資料投稿用（参考資料等）/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleelyk/Documents/Sem7/TecRfidSuiteSample/app/src/main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{19FF92AB-39E7-484D-A150-BE36508958FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C432940-0933-47F5-8E69-D2BFDC4863B0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68778E1E-B04F-BD44-996C-10D09CF37AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="11740" yWindow="3920" windowWidth="7500" windowHeight="8040" activeTab="3" xr2:uid="{CD96D5B0-B126-4985-8F78-41C3AC658D8D}"/>
+    <workbookView xWindow="4960" yWindow="1900" windowWidth="20820" windowHeight="17220" firstSheet="1" activeTab="3" xr2:uid="{CD96D5B0-B126-4985-8F78-41C3AC658D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ｱｲﾃﾑｺｰﾄﾞの基本" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Aptos Narrow"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -296,7 +296,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Aptos Narrow"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -402,7 +402,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Aptos Narrow"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -948,40 +948,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>一方、前回棚卸は2024/3/31とすると、上記のシステムからダウンロードした情報に、「前回棚卸から変動有無」をエクセルで追記。</t>
-    <rPh sb="0" eb="2">
-      <t>イッポウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ゼンカイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>タナオロシ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジョウキ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ゼンカイ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>タナオロシ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヘンドウ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ウム</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ツイキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>前回棚卸</t>
     <rPh sb="0" eb="4">
       <t>ゼンカイタナオロシ</t>
@@ -1256,6 +1222,9 @@
       <t>コ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一方、前回棚卸は2024/3/31とすると、上記のシステムからダウンロードした情報に、「前回棚卸から変動有無」をエクセルで追記。</t>
   </si>
 </sst>
 </file>
@@ -1266,14 +1235,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1281,7 +1250,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1431,7 +1400,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3000,10 +2969,10 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="14" max="14" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
@@ -3176,14 +3145,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE1D23C-3E15-46F9-B932-50A4508B610E}">
   <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
@@ -3329,17 +3298,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07747E66-6D86-4932-8065-15EEAC8F0226}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:F30"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -3485,40 +3454,40 @@
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="F21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" s="2">
         <v>45382</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" ht="18">
       <c r="B22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="9" t="s">
+    </row>
+    <row r="23" spans="2:7" ht="18">
+      <c r="B23" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="D23" s="11">
         <v>10</v>
@@ -3531,15 +3500,15 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="18">
+      <c r="B24" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="D24" s="11">
         <v>50</v>
@@ -3552,12 +3521,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" ht="18">
       <c r="B25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="11">
         <v>100</v>
@@ -3570,12 +3539,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" ht="18">
       <c r="B26" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="D26" s="11">
         <v>0</v>
@@ -3588,12 +3557,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" ht="18">
       <c r="B27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="D27" s="11">
         <v>50</v>
@@ -3606,12 +3575,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" ht="18">
       <c r="B28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="D28" s="11">
         <v>0</v>
@@ -3624,12 +3593,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" ht="18">
       <c r="B29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="D29" s="11">
         <v>0</v>
@@ -3642,12 +3611,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" ht="18">
       <c r="B30" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="D30" s="11">
         <v>60</v>
@@ -3662,12 +3631,12 @@
     </row>
     <row r="33" spans="2:6">
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="2:6">
@@ -3684,7 +3653,7 @@
         <v>53</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -3761,12 +3730,12 @@
     </row>
     <row r="42" spans="2:6">
       <c r="B42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3780,19 +3749,19 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="18.125" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="2" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -3802,37 +3771,37 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>54</v>
@@ -3927,6 +3896,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101009E1C846E12A1F148B870DA000F4FEE94" ma:contentTypeVersion="8" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="ddb4a35e8bb218006082b4c41c5287cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0ce453c-4a97-466a-bfbe-896b911d08cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20129c816e42a14b43849ca959e7bc96" ns2:_="">
     <xsd:import namespace="f0ce453c-4a97-466a-bfbe-896b911d08cf"/>
@@ -4094,20 +4069,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A387AE-1F3E-4CCA-B774-A7E3AFFEB501}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A387AE-1F3E-4CCA-B774-A7E3AFFEB501}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC1238BF-EF4B-405A-ACE8-F66248A9B950}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F87A85-6FDD-45C8-B6F2-0AC70345EAF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F87A85-6FDD-45C8-B6F2-0AC70345EAF9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC1238BF-EF4B-405A-ACE8-F66248A9B950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0ce453c-4a97-466a-bfbe-896b911d08cf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Jig search UI added
</commit_message>
<xml_diff>
--- a/app/src/main/assets/RFID_file.xlsx
+++ b/app/src/main/assets/RFID_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleelyk/Documents/Sem7/TecRfidSuiteSample/app/src/main/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68778E1E-B04F-BD44-996C-10D09CF37AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CA88B0-B755-9E4F-8AAD-708306F6FE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="1900" windowWidth="20820" windowHeight="17220" firstSheet="1" activeTab="3" xr2:uid="{CD96D5B0-B126-4985-8F78-41C3AC658D8D}"/>
+    <workbookView xWindow="2360" yWindow="1200" windowWidth="21220" windowHeight="17220" firstSheet="1" activeTab="2" xr2:uid="{CD96D5B0-B126-4985-8F78-41C3AC658D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ｱｲﾃﾑｺｰﾄﾞの基本" sheetId="1" r:id="rId1"/>
@@ -3298,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07747E66-6D86-4932-8065-15EEAC8F0226}">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="92" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3553,8 +3553,7 @@
         <v>45463</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="18">
@@ -3571,8 +3570,7 @@
         <v>43958</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="18">
@@ -3706,8 +3704,7 @@
         <v>45463</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -3748,8 +3745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8998224E-62D6-4D86-811A-54D5408F8AEB}">
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A2" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3896,12 +3893,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101009E1C846E12A1F148B870DA000F4FEE94" ma:contentTypeVersion="8" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="ddb4a35e8bb218006082b4c41c5287cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0ce453c-4a97-466a-bfbe-896b911d08cf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20129c816e42a14b43849ca959e7bc96" ns2:_="">
     <xsd:import namespace="f0ce453c-4a97-466a-bfbe-896b911d08cf"/>
@@ -4069,6 +4060,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A387AE-1F3E-4CCA-B774-A7E3AFFEB501}">
   <ds:schemaRefs>
@@ -4078,15 +4075,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F87A85-6FDD-45C8-B6F2-0AC70345EAF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC1238BF-EF4B-405A-ACE8-F66248A9B950}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4102,4 +4090,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F87A85-6FDD-45C8-B6F2-0AC70345EAF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>